<commit_message>
K-means clustering based on RFM
</commit_message>
<xml_diff>
--- a/final_clean_data_dictionary.xlsx
+++ b/final_clean_data_dictionary.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Behzad\Documents\GitHub\Telecom_Churn\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C0E31-E9BD-4760-BD40-4917675D6B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1120,8 +1139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1184,13 +1203,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1228,7 +1255,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1262,6 +1289,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1296,9 +1324,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1471,14 +1500,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1503,7 +1537,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1514,7 +1548,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1559,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1536,7 +1570,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1547,7 +1581,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1558,7 +1592,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1606,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1586,7 +1620,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1600,7 +1634,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1614,7 +1648,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1662,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1642,7 +1676,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1656,7 +1690,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1670,7 +1704,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1684,7 +1718,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1698,7 +1732,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1712,7 +1746,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1726,7 +1760,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1740,7 +1774,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1788,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1768,7 +1802,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1782,7 +1816,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1796,7 +1830,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1810,7 +1844,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1824,7 +1858,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1838,7 +1872,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1852,7 +1886,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1866,7 +1900,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1880,7 +1914,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1894,7 +1928,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1908,7 +1942,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1922,7 +1956,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1936,7 +1970,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1950,7 +1984,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1964,7 +1998,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1978,7 +2012,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1992,7 +2026,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2006,7 +2040,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2020,7 +2054,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -2034,7 +2068,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2048,7 +2082,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2062,7 +2096,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2076,7 +2110,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2090,7 +2124,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -2104,7 +2138,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2118,7 +2152,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2132,7 +2166,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2146,7 +2180,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -2160,7 +2194,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2174,7 +2208,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2188,7 +2222,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -2202,7 +2236,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -2216,7 +2250,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -2230,7 +2264,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -2244,7 +2278,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -2258,7 +2292,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -2272,7 +2306,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2286,7 +2320,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -2300,7 +2334,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -2314,7 +2348,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -2328,7 +2362,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -2342,7 +2376,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -2356,7 +2390,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -2370,7 +2404,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -2384,7 +2418,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2398,7 +2432,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2412,7 +2446,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -2426,7 +2460,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -2440,7 +2474,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -2454,7 +2488,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -2468,7 +2502,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -2482,7 +2516,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -2496,7 +2530,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -2510,7 +2544,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -2524,7 +2558,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -2538,7 +2572,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -2552,7 +2586,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -2566,7 +2600,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -2580,7 +2614,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -2594,7 +2628,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -2608,7 +2642,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -2622,7 +2656,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -2636,7 +2670,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -2650,7 +2684,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -2664,7 +2698,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>89</v>
       </c>
@@ -2678,7 +2712,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -2692,7 +2726,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>91</v>
       </c>
@@ -2706,7 +2740,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -2720,7 +2754,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>93</v>
       </c>
@@ -2734,7 +2768,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -2748,7 +2782,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -2762,7 +2796,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -2776,7 +2810,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -2790,7 +2824,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -2804,7 +2838,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -2818,7 +2852,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -2832,7 +2866,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -2846,7 +2880,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -2860,7 +2894,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -2874,7 +2908,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -2888,7 +2922,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -2902,7 +2936,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -2916,7 +2950,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -2930,7 +2964,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -2944,7 +2978,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -2958,7 +2992,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -2972,7 +3006,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -2986,7 +3020,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -3000,7 +3034,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>113</v>
       </c>
@@ -3014,7 +3048,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>114</v>
       </c>
@@ -3028,7 +3062,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>115</v>
       </c>
@@ -3042,7 +3076,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>116</v>
       </c>
@@ -3056,7 +3090,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>117</v>
       </c>
@@ -3070,7 +3104,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>118</v>
       </c>
@@ -3084,7 +3118,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>119</v>
       </c>
@@ -3098,7 +3132,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -3112,7 +3146,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -3126,7 +3160,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>122</v>
       </c>
@@ -3140,7 +3174,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>123</v>
       </c>
@@ -3154,7 +3188,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>124</v>
       </c>
@@ -3168,7 +3202,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>125</v>
       </c>
@@ -3182,7 +3216,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>126</v>
       </c>
@@ -3193,7 +3227,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>127</v>
       </c>
@@ -3204,7 +3238,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>128</v>
       </c>
@@ -3215,7 +3249,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>129</v>
       </c>
@@ -3226,7 +3260,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>130</v>
       </c>
@@ -3240,7 +3274,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>131</v>
       </c>
@@ -3254,7 +3288,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>132</v>
       </c>
@@ -3268,7 +3302,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>133</v>
       </c>
@@ -3282,7 +3316,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>134</v>
       </c>
@@ -3296,7 +3330,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>135</v>
       </c>
@@ -3310,7 +3344,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>136</v>
       </c>
@@ -3324,7 +3358,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>137</v>
       </c>
@@ -3338,7 +3372,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>138</v>
       </c>
@@ -3352,7 +3386,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>139</v>
       </c>
@@ -3366,7 +3400,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>140</v>
       </c>
@@ -3380,7 +3414,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>141</v>
       </c>
@@ -3394,7 +3428,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>142</v>
       </c>
@@ -3408,7 +3442,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>143</v>
       </c>
@@ -3422,7 +3456,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>144</v>
       </c>
@@ -3436,7 +3470,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>145</v>
       </c>
@@ -3450,7 +3484,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>146</v>
       </c>
@@ -3464,7 +3498,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>147</v>
       </c>
@@ -3478,7 +3512,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>148</v>
       </c>
@@ -3492,7 +3526,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>149</v>
       </c>
@@ -3506,7 +3540,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>150</v>
       </c>
@@ -3520,7 +3554,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>151</v>
       </c>
@@ -3534,7 +3568,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>152</v>
       </c>
@@ -3548,7 +3582,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>153</v>
       </c>
@@ -3562,7 +3596,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>154</v>
       </c>
@@ -3576,7 +3610,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>155</v>
       </c>
@@ -3590,7 +3624,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>156</v>
       </c>
@@ -3604,7 +3638,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>157</v>
       </c>
@@ -3618,7 +3652,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>158</v>
       </c>
@@ -3632,7 +3666,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>159</v>
       </c>
@@ -3646,7 +3680,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>160</v>
       </c>
@@ -3660,7 +3694,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -3674,7 +3708,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>162</v>
       </c>
@@ -3688,7 +3722,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>163</v>
       </c>
@@ -3702,7 +3736,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>164</v>
       </c>
@@ -3716,7 +3750,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>165</v>
       </c>
@@ -3730,7 +3764,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>166</v>
       </c>
@@ -3744,7 +3778,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>167</v>
       </c>
@@ -3758,7 +3792,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>168</v>
       </c>
@@ -3772,7 +3806,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>169</v>
       </c>
@@ -3786,7 +3820,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>170</v>
       </c>
@@ -3800,7 +3834,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>171</v>
       </c>
@@ -3814,7 +3848,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>172</v>
       </c>
@@ -3828,7 +3862,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>173</v>
       </c>
@@ -3842,7 +3876,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>174</v>
       </c>
@@ -3856,7 +3890,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>175</v>
       </c>
@@ -3870,7 +3904,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>176</v>
       </c>
@@ -3884,7 +3918,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>177</v>
       </c>
@@ -3898,7 +3932,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>178</v>
       </c>
@@ -3912,7 +3946,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>179</v>
       </c>
@@ -3926,7 +3960,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>180</v>
       </c>
@@ -3940,7 +3974,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>181</v>
       </c>
@@ -3954,7 +3988,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>182</v>
       </c>
@@ -3968,7 +4002,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>183</v>
       </c>
@@ -3982,7 +4016,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>184</v>
       </c>
@@ -3996,7 +4030,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>185</v>
       </c>
@@ -4010,7 +4044,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>186</v>
       </c>
@@ -4024,7 +4058,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>187</v>
       </c>
@@ -4038,7 +4072,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>188</v>
       </c>

</xml_diff>